<commit_message>
Added a lot of changes to dissertation
Trying to streamline the sentiment analysis
</commit_message>
<xml_diff>
--- a/dissertation/saTests/twinPeaksData.xlsx
+++ b/dissertation/saTests/twinPeaksData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markb\Documents\GitHub\uniWork\dissertation\saTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2282BEF1-4E6D-4C5C-9B29-D21245FF5ED3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C739A5-9E2F-44F3-B31C-7C2B69304BE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="17280" windowHeight="8964" xr2:uid="{A2F98D7D-73BE-49C7-AAAC-B193CEB33A64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>imdb-rating</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>u.s-viewers-millions</t>
+  </si>
+  <si>
+    <t>sentiment-affin-sum</t>
   </si>
 </sst>
 </file>
@@ -233,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,6 +326,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5338,16 +5344,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>20280</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>12660</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>119575</xdr:rowOff>
+      <xdr:rowOff>81475</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5782,10 +5788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CCAD1F-C37B-4DA9-8C2A-89122FB84B64}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5796,9 +5802,10 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
@@ -5817,8 +5824,11 @@
       <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="31" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -5837,8 +5847,11 @@
       <c r="F2" s="12">
         <v>34.6</v>
       </c>
+      <c r="G2" s="14">
+        <v>433</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -5858,7 +5871,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -5878,7 +5891,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -5898,7 +5911,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>1</v>
       </c>
@@ -5918,7 +5931,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>1</v>
       </c>
@@ -5938,7 +5951,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>1</v>
       </c>
@@ -5958,7 +5971,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>1</v>
       </c>
@@ -5978,7 +5991,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -5998,7 +6011,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -6018,7 +6031,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -6038,7 +6051,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -6058,7 +6071,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2</v>
       </c>
@@ -6078,7 +6091,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2</v>
       </c>
@@ -6098,7 +6111,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>2</v>
       </c>

</xml_diff>